<commit_message>
few changes (not usefull)
</commit_message>
<xml_diff>
--- a/mesures_couverts.xlsx
+++ b/mesures_couverts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maral\Desktop\Universite\MASTER1\Q2\LBIRA2130 - Projet disciplinaire\LBIRA2130_Couverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DA2EBD-9E70-4275-BDB6-82B005F96760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD504281-11EF-4B38-AB5F-1F41C5607EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D0C76E02-6240-421E-9415-499825F072BD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="65">
   <si>
     <t>ID_planche</t>
   </si>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206F8975-33D2-4BAA-996D-101D2A201CBE}">
   <dimension ref="A1:AA501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,18 +820,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>60</v>
-      </c>
+      <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -859,18 +853,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -898,18 +886,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -941,9 +923,7 @@
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -976,9 +956,7 @@
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1011,9 +989,7 @@
       <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1046,9 +1022,7 @@
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1081,9 +1055,7 @@
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1116,9 +1088,7 @@
       <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1151,9 +1121,7 @@
       <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1186,9 +1154,7 @@
       <c r="D12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1221,9 +1187,7 @@
       <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1256,9 +1220,7 @@
       <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1291,9 +1253,7 @@
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1326,9 +1286,7 @@
       <c r="D16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1361,9 +1319,7 @@
       <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1396,9 +1352,7 @@
       <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1431,9 +1385,7 @@
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1466,9 +1418,7 @@
       <c r="D20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1501,9 +1451,7 @@
       <c r="D21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>

</xml_diff>